<commit_message>
mise à jour backend avec yolo
</commit_message>
<xml_diff>
--- a/exports/releve_01.xlsx
+++ b/exports/releve_01.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Banque</t>
   </si>
@@ -49,13 +49,25 @@
     <t>Sens</t>
   </si>
   <si>
+    <t>01/04/2019</t>
+  </si>
+  <si>
+    <t>STATEMENT BETWEEN AND FOR A/C: 918020087855304 (589) MS. INNOVAGION AIR CONDITIONING KH. NO 27! 8-69 UDAY VIHAR NILOTHIEXTN,, WEST OELMI DELHI POOJA DAIRY DELHI DELHI NO PIN: 110081 ‘SCHEME CODE ‘OA- LARGE RETAILERS AND DISTRIBUTORS ‘CUSTOMER 1D 985641520 CURRENCY. CODE INR, (WEN AMOUNT NOMINATION DETAILS — : NOMINATION REGISTERED ‘Tran Date | Value Date | Transaction Details [ohq. NoJAmount (in Rs.)JOr/Cr] Balance (ins) [Branch Name TOOTS | TOONS 7] TORR NAGAR raoazore | 19082010 | 3202881 | TILAK NAGAR rsoa2or8 [ 19082019 750] Dr 0438.81 TILAK NAGAR TTOE2OTO_|_17OUZOTO. T2005.00] — Or 7432.91] TAK NAGAR [enoxeors | eooazore 71000] — or Bio | —TICAR NAGAR zooazore | 20082019 2680] 0 Tes2.91 | TAK NAGAR zooazore | 220a2019 448.00] 0 ‘91[ TILAK NAGAR | 2042010 | -2570472019_ [RTGSIICIGHTOTIS9077S5SUZUKIMOTO. "3E2TO| — cr Besse. 91| GANGA Pa] GEOEGOIS | SO10W/G0TO |NEFTINGIANNETSTTOO Sa06DIchots 7511.00] Or 2ans7s01] MONGAIFORT</t>
+  </si>
+  <si>
+    <t>0.00</t>
+  </si>
+  <si>
+    <t>Cr</t>
+  </si>
+  <si>
     <t>20/04/2019</t>
   </si>
   <si>
-    <t>25042018 [ |NEFTMEVAXME1611907@0861/Gurmest  Dr 73957391 | BHAWANIPATIT</t>
-  </si>
-  <si>
-    <t>7750000.00</t>
+    <t>25042018 [ |NEFTMEVAXME1611907@0861/Gurmest 7750 Dr 73957391 | BHAWANIPATIT zaoaz019 | 207042019 |MOBISELFFTISURJEET SINGH/S130100 Dy 190373.91 | — TILAK NAGAR LI T-SIe VIRASPURIOELATIOO 7 TOOTS | GOONS oy TISESBOT] — TILAK NAGAR. TRANSACTION TOTAL DRICR: 309687.00 CLOSING BALANCE : ane 11596801</t>
+  </si>
+  <si>
+    <t>000.00</t>
   </si>
   <si>
     <t>Dr</t>
@@ -390,7 +402,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -453,6 +465,20 @@
         <v>14</v>
       </c>
     </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>